<commit_message>
Improving MultiIndex Slicing Support
</commit_message>
<xml_diff>
--- a/MultiIndexCase.xlsx
+++ b/MultiIndexCase.xlsx
@@ -34,10 +34,16 @@
     <t>Weds</t>
   </si>
   <si>
+    <t>Post-Noon</t>
+  </si>
+  <si>
     <t>Pre-Noon</t>
   </si>
   <si>
-    <t>Post-Noon</t>
+    <t>Dinner</t>
+  </si>
+  <si>
+    <t>Midnight Snack</t>
   </si>
   <si>
     <t>Breakfast</t>
@@ -46,10 +52,10 @@
     <t>Lunch</t>
   </si>
   <si>
-    <t>Dinner</t>
-  </si>
-  <si>
-    <t>Midnight Snack</t>
+    <t>Curry</t>
+  </si>
+  <si>
+    <t>Shmores</t>
   </si>
   <si>
     <t>Toast</t>
@@ -58,16 +64,10 @@
     <t>Soup</t>
   </si>
   <si>
-    <t>Curry</t>
-  </si>
-  <si>
-    <t>Shmores</t>
+    <t>Chocolate</t>
   </si>
   <si>
     <t>Hotpot</t>
-  </si>
-  <si>
-    <t>Chocolate</t>
   </si>
   <si>
     <t>Something Different!</t>
@@ -495,10 +495,10 @@
         <v>16</v>
       </c>
       <c r="M9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="N9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="9:14">
@@ -533,10 +533,10 @@
         <v>17</v>
       </c>
       <c r="M11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" t="s">
         <v>15</v>
-      </c>
-      <c r="N11" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>